<commit_message>
Correcting minor mistakes in (a) score range of Meta-SVM (1 out of 31 tools used), resulting in minor changes in Figure 5 and Suppl Files 2 and 3 (b) y-axis for SpliceAI in Figure 5 (no change in actual data). The changes do not change any of the the outcomes of the study.
</commit_message>
<xml_diff>
--- a/plots/plot-source-files/Figure-5-S1-data.xlsx
+++ b/plots/plot-source-files/Figure-5-S1-data.xlsx
@@ -550,7 +550,7 @@
         <v>13</v>
       </c>
       <c r="C31" t="n">
-        <v>98.0</v>
+        <v>56.0</v>
       </c>
       <c r="D31" t="s">
         <v>17</v>
@@ -564,7 +564,7 @@
         <v>14</v>
       </c>
       <c r="C32" t="n">
-        <v>371.0</v>
+        <v>413.0</v>
       </c>
       <c r="D32" t="s">
         <v>18</v>

</xml_diff>